<commit_message>
updated files updated file loader
</commit_message>
<xml_diff>
--- a/dls_set/EDR_05/cycle6/2.xlsx
+++ b/dls_set/EDR_05/cycle6/2.xlsx
@@ -88,10 +88,10 @@
         <v>0.53366994857788086</v>
       </c>
       <c r="B2" s="0">
-        <v>37.899875640869141</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>92.835357666015625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -99,10 +99,10 @@
         <v>0.61359071731567383</v>
       </c>
       <c r="B3" s="0">
-        <v>36.867225646972656</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0">
-        <v>90.3058853149414</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -110,10 +110,10 @@
         <v>0.70548021793365479</v>
       </c>
       <c r="B4" s="0">
-        <v>35.834575653076172</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>87.776420593261719</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -121,10 +121,10 @@
         <v>0.8111308217048645</v>
       </c>
       <c r="B5" s="0">
-        <v>34.801925659179688</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0">
-        <v>85.246955871582031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -132,10 +132,10 @@
         <v>0.93260329961776733</v>
       </c>
       <c r="B6" s="0">
-        <v>33.769271850585938</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>82.717491149902344</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -143,10 +143,10 @@
         <v>1.0722672939300537</v>
       </c>
       <c r="B7" s="0">
-        <v>32.736621856689453</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0">
-        <v>80.188026428222656</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -154,10 +154,10 @@
         <v>1.232846736907959</v>
       </c>
       <c r="B8" s="0">
-        <v>31.703971862792969</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0">
-        <v>77.658554077148438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -165,10 +165,10 @@
         <v>1.4174741506576538</v>
       </c>
       <c r="B9" s="0">
-        <v>30.671321868896484</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0">
-        <v>75.12908935546875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -176,10 +176,10 @@
         <v>1.6297508478164673</v>
       </c>
       <c r="B10" s="0">
-        <v>29.638671875</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0">
-        <v>72.599624633789063</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -187,10 +187,10 @@
         <v>1.8738173246383667</v>
       </c>
       <c r="B11" s="0">
-        <v>28.606021881103516</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0">
-        <v>70.070152282714844</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -198,10 +198,10 @@
         <v>2.1544346809387207</v>
       </c>
       <c r="B12" s="0">
-        <v>27.573371887207031</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>67.540687561035156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -209,10 +209,10 @@
         <v>2.4770762920379639</v>
       </c>
       <c r="B13" s="0">
-        <v>26.540719985961914</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>65.011222839355469</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -220,10 +220,10 @@
         <v>2.8480358123779297</v>
       </c>
       <c r="B14" s="0">
-        <v>25.545866012573242</v>
+        <v>0.045353539288043976</v>
       </c>
       <c r="C14" s="0">
-        <v>62.463272094726563</v>
+        <v>0.070209339261054993</v>
       </c>
     </row>
     <row r="15">
@@ -231,10 +231,10 @@
         <v>3.2745490074157715</v>
       </c>
       <c r="B15" s="0">
-        <v>24.927194595336914</v>
+        <v>0.54213064908981323</v>
       </c>
       <c r="C15" s="0">
-        <v>59.731353759765625</v>
+        <v>0.24002590775489807</v>
       </c>
     </row>
     <row r="16">
@@ -242,10 +242,10 @@
         <v>3.7649359703063965</v>
       </c>
       <c r="B16" s="0">
-        <v>24.95672607421875</v>
+        <v>1.8167499303817749</v>
       </c>
       <c r="C16" s="0">
-        <v>56.681705474853516</v>
+        <v>0.28282567858695984</v>
       </c>
     </row>
     <row r="17">
@@ -253,10 +253,10 @@
         <v>4.3287615776062012</v>
       </c>
       <c r="B17" s="0">
-        <v>25.406827926635742</v>
+        <v>3.5960521697998047</v>
       </c>
       <c r="C17" s="0">
-        <v>53.428237915039063</v>
+        <v>0.62914460897445679</v>
       </c>
     </row>
     <row r="18">
@@ -264,10 +264,10 @@
         <v>4.9770236015319824</v>
       </c>
       <c r="B18" s="0">
-        <v>25.843963623046875</v>
+        <v>5.3597936630249023</v>
       </c>
       <c r="C18" s="0">
-        <v>50.1877555847168</v>
+        <v>1.2266266345977783</v>
       </c>
     </row>
     <row r="19">
@@ -275,10 +275,10 @@
         <v>5.7223672866821289</v>
       </c>
       <c r="B19" s="0">
-        <v>25.847869873046875</v>
+        <v>6.603663444519043</v>
       </c>
       <c r="C19" s="0">
-        <v>47.164340972900391</v>
+        <v>1.7457572221755981</v>
       </c>
     </row>
     <row r="20">
@@ -286,10 +286,10 @@
         <v>6.57933235168457</v>
       </c>
       <c r="B20" s="0">
-        <v>25.150234222412109</v>
+        <v>7.0056796073913574</v>
       </c>
       <c r="C20" s="0">
-        <v>44.480232238769531</v>
+        <v>1.9818108081817627</v>
       </c>
     </row>
     <row r="21">
@@ -297,10 +297,10 @@
         <v>7.5646333694458008</v>
       </c>
       <c r="B21" s="0">
-        <v>23.695043563842773</v>
+        <v>6.4986319541931152</v>
       </c>
       <c r="C21" s="0">
-        <v>42.155357360839844</v>
+        <v>1.8624374866485596</v>
       </c>
     </row>
     <row r="22">
@@ -308,10 +308,10 @@
         <v>8.6974897384643555</v>
       </c>
       <c r="B22" s="0">
-        <v>21.630632400512695</v>
+        <v>5.2605199813842773</v>
       </c>
       <c r="C22" s="0">
-        <v>40.119464874267578</v>
+        <v>1.4526060819625854</v>
       </c>
     </row>
     <row r="23">
@@ -319,10 +319,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="0">
-        <v>19.249584197998047</v>
+        <v>3.6424412727355957</v>
       </c>
       <c r="C23" s="0">
-        <v>38.238594055175781</v>
+        <v>0.93047523498535156</v>
       </c>
     </row>
     <row r="24">
@@ -330,10 +330,10 @@
         <v>11.497570037841797</v>
       </c>
       <c r="B24" s="0">
-        <v>16.896551132202148</v>
+        <v>2.0579819679260254</v>
       </c>
       <c r="C24" s="0">
-        <v>36.350120544433594</v>
+        <v>0.53905999660491943</v>
       </c>
     </row>
     <row r="25">
@@ -341,10 +341,10 @@
         <v>13.21941089630127</v>
       </c>
       <c r="B25" s="0">
-        <v>14.864974975585938</v>
+        <v>0.85927265882492065</v>
       </c>
       <c r="C25" s="0">
-        <v>34.308673858642578</v>
+        <v>0.39832442998886108</v>
       </c>
     </row>
     <row r="26">
@@ -352,10 +352,10 @@
         <v>15.199110984802246</v>
       </c>
       <c r="B26" s="0">
-        <v>13.301700592041016</v>
+        <v>0.22252239286899567</v>
       </c>
       <c r="C26" s="0">
-        <v>32.038234710693359</v>
+        <v>0.27227833867073059</v>
       </c>
     </row>
     <row r="27">
@@ -363,10 +363,10 @@
         <v>17.475282669067383</v>
       </c>
       <c r="B27" s="0">
-        <v>12.134117126464844</v>
+        <v>0.06060342863202095</v>
       </c>
       <c r="C27" s="0">
-        <v>29.574039459228516</v>
+        <v>0.083006061613559723</v>
       </c>
     </row>
     <row r="28">
@@ -374,10 +374,10 @@
         <v>20.092329025268555</v>
       </c>
       <c r="B28" s="0">
-        <v>11.073648452758789</v>
+        <v>0.027220681309700012</v>
       </c>
       <c r="C28" s="0">
-        <v>27.058168411254883</v>
+        <v>0.060867298394441605</v>
       </c>
     </row>
     <row r="29">
@@ -385,10 +385,10 @@
         <v>23.101297378540039</v>
       </c>
       <c r="B29" s="0">
-        <v>10.052036285400391</v>
+        <v>0.040450219064950943</v>
       </c>
       <c r="C29" s="0">
-        <v>24.523410797119141</v>
+        <v>0.090449444949626923</v>
       </c>
     </row>
     <row r="30">
@@ -396,10 +396,10 @@
         <v>26.560878753662109</v>
       </c>
       <c r="B30" s="0">
-        <v>9.03262710571289</v>
+        <v>0.056257877498865128</v>
       </c>
       <c r="C30" s="0">
-        <v>21.987813949584961</v>
+        <v>0.12579643726348877</v>
       </c>
     </row>
     <row r="31">
@@ -407,10 +407,10 @@
         <v>30.538555145263672</v>
       </c>
       <c r="B31" s="0">
-        <v>8.0642032623291016</v>
+        <v>0.1329600065946579</v>
       </c>
       <c r="C31" s="0">
-        <v>19.427833557128906</v>
+        <v>0.12701381742954254</v>
       </c>
     </row>
     <row r="32">
@@ -418,10 +418,10 @@
         <v>35.111915588378906</v>
       </c>
       <c r="B32" s="0">
-        <v>7.1835746765136719</v>
+        <v>0.31399592757225037</v>
       </c>
       <c r="C32" s="0">
-        <v>16.827726364135742</v>
+        <v>0.17910207808017731</v>
       </c>
     </row>
     <row r="33">
@@ -429,10 +429,10 @@
         <v>40.370170593261719</v>
       </c>
       <c r="B33" s="0">
-        <v>6.348078727722168</v>
+        <v>0.5460735559463501</v>
       </c>
       <c r="C33" s="0">
-        <v>14.21497631072998</v>
+        <v>0.32781586050987244</v>
       </c>
     </row>
     <row r="34">
@@ -440,10 +440,10 @@
         <v>46.415889739990234</v>
       </c>
       <c r="B34" s="0">
-        <v>5.4909896850585938</v>
+        <v>0.74393594264984131</v>
       </c>
       <c r="C34" s="0">
-        <v>11.635554313659668</v>
+        <v>0.47304326295852661</v>
       </c>
     </row>
     <row r="35">
@@ -451,10 +451,10 @@
         <v>53.366992950439453</v>
       </c>
       <c r="B35" s="0">
-        <v>4.5642685890197754</v>
+        <v>0.83866149187088013</v>
       </c>
       <c r="C35" s="0">
-        <v>9.1392154693603516</v>
+        <v>0.5527070164680481</v>
       </c>
     </row>
     <row r="36">
@@ -462,10 +462,10 @@
         <v>61.359073638916016</v>
       </c>
       <c r="B36" s="0">
-        <v>3.5650293827056885</v>
+        <v>0.80513209104537964</v>
       </c>
       <c r="C36" s="0">
-        <v>6.7782630920410156</v>
+        <v>0.55073446035385132</v>
       </c>
     </row>
     <row r="37">
@@ -473,10 +473,10 @@
         <v>70.548027038574219</v>
       </c>
       <c r="B37" s="0">
-        <v>2.544522762298584</v>
+        <v>0.66804289817810059</v>
       </c>
       <c r="C37" s="0">
-        <v>4.617042064666748</v>
+        <v>0.4873606264591217</v>
       </c>
     </row>
     <row r="38">
@@ -484,10 +484,10 @@
         <v>81.113082885742188</v>
       </c>
       <c r="B38" s="0">
-        <v>1.5996847152709961</v>
+        <v>0.48890575766563416</v>
       </c>
       <c r="C38" s="0">
-        <v>2.7445995807647705</v>
+        <v>0.40287584066390991</v>
       </c>
     </row>
     <row r="39">
@@ -495,10 +495,10 @@
         <v>93.260330200195313</v>
       </c>
       <c r="B39" s="0">
-        <v>0.84716182947158813</v>
+        <v>0.33851951360702515</v>
       </c>
       <c r="C39" s="0">
-        <v>1.2829173803329468</v>
+        <v>0.34200698137283325</v>
       </c>
     </row>
     <row r="40">
@@ -506,10 +506,10 @@
         <v>107.22672271728516</v>
       </c>
       <c r="B40" s="0">
-        <v>0.37823566794395447</v>
+        <v>0.26021048426628113</v>
       </c>
       <c r="C40" s="0">
-        <v>0.42118048667907715</v>
+        <v>0.34244221448898315</v>
       </c>
     </row>
     <row r="41">
@@ -517,10 +517,10 @@
         <v>123.28467559814453</v>
       </c>
       <c r="B41" s="0">
-        <v>0.19075010716915131</v>
+        <v>0.22890013456344604</v>
       </c>
       <c r="C41" s="0">
-        <v>0.37295868992805481</v>
+        <v>0.40367940068244934</v>
       </c>
     </row>
     <row r="42">
@@ -528,10 +528,10 @@
         <v>141.74742126464844</v>
       </c>
       <c r="B42" s="0">
-        <v>0.17971119284629822</v>
+        <v>0.21565344929695129</v>
       </c>
       <c r="C42" s="0">
-        <v>0.41656345129013062</v>
+        <v>0.45521152019500732</v>
       </c>
     </row>
     <row r="43">
@@ -539,10 +539,10 @@
         <v>162.97508239746094</v>
       </c>
       <c r="B43" s="0">
-        <v>0.16989597678184509</v>
+        <v>0.20387516915798187</v>
       </c>
       <c r="C43" s="0">
-        <v>0.41615846753120422</v>
+        <v>0.45587876439094543</v>
       </c>
     </row>
     <row r="44">
@@ -550,10 +550,10 @@
         <v>187.38174438476563</v>
       </c>
       <c r="B44" s="0">
-        <v>0.15083052217960358</v>
+        <v>0.1809966117143631</v>
       </c>
       <c r="C44" s="0">
-        <v>0.36945781111717224</v>
+        <v>0.40472075343132019</v>
       </c>
     </row>
     <row r="45">
@@ -561,10 +561,10 @@
         <v>215.44346618652344</v>
       </c>
       <c r="B45" s="0">
-        <v>0.118693046271801</v>
+        <v>0.14243166148662567</v>
       </c>
       <c r="C45" s="0">
-        <v>0.29073742032051086</v>
+        <v>0.31848686933517456</v>
       </c>
     </row>
     <row r="46">
@@ -572,10 +572,10 @@
         <v>247.7076416015625</v>
       </c>
       <c r="B46" s="0">
-        <v>0.08071570098400116</v>
+        <v>0.096858836710453033</v>
       </c>
       <c r="C46" s="0">
-        <v>0.19771228730678558</v>
+        <v>0.21658295392990112</v>
       </c>
     </row>
     <row r="47">
@@ -583,10 +583,10 @@
         <v>284.8035888671875</v>
       </c>
       <c r="B47" s="0">
-        <v>0.045013111084699631</v>
+        <v>0.054015733301639557</v>
       </c>
       <c r="C47" s="0">
-        <v>0.11025915294885635</v>
+        <v>0.12078285217285156</v>
       </c>
     </row>
     <row r="48">
@@ -594,10 +594,10 @@
         <v>327.45492553710938</v>
       </c>
       <c r="B48" s="0">
-        <v>0.0182975921779871</v>
+        <v>0.021957110613584518</v>
       </c>
       <c r="C48" s="0">
-        <v>0.04481976106762886</v>
+        <v>0.049097590148448944</v>
       </c>
     </row>
     <row r="49">
@@ -605,10 +605,10 @@
         <v>376.49356079101563</v>
       </c>
       <c r="B49" s="0">
-        <v>0.010404767468571663</v>
+        <v>0.01248572114855051</v>
       </c>
       <c r="C49" s="0">
-        <v>0.016950780525803566</v>
+        <v>0.018074385821819305</v>
       </c>
     </row>
     <row r="50">
@@ -616,10 +616,10 @@
         <v>432.87612915039063</v>
       </c>
       <c r="B50" s="0">
-        <v>0.022706251591444016</v>
+        <v>0.027247501537203789</v>
       </c>
       <c r="C50" s="0">
-        <v>0.055618729442358017</v>
+        <v>0.060927268117666245</v>
       </c>
     </row>
     <row r="51">
@@ -627,10 +627,10 @@
         <v>497.70233154296875</v>
       </c>
       <c r="B51" s="0">
-        <v>0.042341046035289764</v>
+        <v>0.050809253007173538</v>
       </c>
       <c r="C51" s="0">
-        <v>0.10371395945549011</v>
+        <v>0.11361294984817505</v>
       </c>
     </row>
     <row r="52">
@@ -638,10 +638,10 @@
         <v>572.23681640625</v>
       </c>
       <c r="B52" s="0">
-        <v>0.056758314371109009</v>
+        <v>0.068109974265098572</v>
       </c>
       <c r="C52" s="0">
-        <v>0.13902890682220459</v>
+        <v>0.15229853987693787</v>
       </c>
     </row>
     <row r="53">
@@ -649,10 +649,10 @@
         <v>657.9332275390625</v>
       </c>
       <c r="B53" s="0">
-        <v>0.061259739100933075</v>
+        <v>0.073511689901351929</v>
       </c>
       <c r="C53" s="0">
-        <v>0.14467786252498627</v>
+        <v>0.15823647379875183</v>
       </c>
     </row>
     <row r="54">
@@ -660,10 +660,10 @@
         <v>756.46337890625</v>
       </c>
       <c r="B54" s="0">
-        <v>0.064203798770904541</v>
+        <v>0.077044554054737091</v>
       </c>
       <c r="C54" s="0">
-        <v>0.11756712198257446</v>
+        <v>0.12665265798568726</v>
       </c>
     </row>
     <row r="55">
@@ -671,10 +671,10 @@
         <v>869.74896240234375</v>
       </c>
       <c r="B55" s="0">
-        <v>0.090950444340705872</v>
+        <v>0.10914053022861481</v>
       </c>
       <c r="C55" s="0">
-        <v>0.11588018387556076</v>
+        <v>0.11959797888994217</v>
       </c>
     </row>
     <row r="56">
@@ -682,10 +682,10 @@
         <v>1000</v>
       </c>
       <c r="B56" s="0">
-        <v>0.1871325820684433</v>
+        <v>0.22455909848213196</v>
       </c>
       <c r="C56" s="0">
-        <v>0.23736371099948883</v>
+        <v>0.24478836357593536</v>
       </c>
     </row>
     <row r="57">
@@ -693,10 +693,10 @@
         <v>1149.7569580078125</v>
       </c>
       <c r="B57" s="0">
-        <v>0.41367211937904358</v>
+        <v>0.49640658497810364</v>
       </c>
       <c r="C57" s="0">
-        <v>0.44236788153648376</v>
+        <v>0.43962976336479187</v>
       </c>
     </row>
     <row r="58">
@@ -704,10 +704,10 @@
         <v>1321.941162109375</v>
       </c>
       <c r="B58" s="0">
-        <v>0.7529798150062561</v>
+        <v>0.90357577800750732</v>
       </c>
       <c r="C58" s="0">
-        <v>0.71233290433883667</v>
+        <v>0.68130695819854736</v>
       </c>
     </row>
     <row r="59">
@@ -715,10 +715,10 @@
         <v>1519.9110107421875</v>
       </c>
       <c r="B59" s="0">
-        <v>1.1168121099472046</v>
+        <v>1.3401745557785034</v>
       </c>
       <c r="C59" s="0">
-        <v>1.0340614318847656</v>
+        <v>0.98103153705596924</v>
       </c>
     </row>
     <row r="60">
@@ -726,10 +726,10 @@
         <v>1747.5283203125</v>
       </c>
       <c r="B60" s="0">
-        <v>1.4124419689178467</v>
+        <v>1.6949303150177002</v>
       </c>
       <c r="C60" s="0">
-        <v>1.3744739294052124</v>
+        <v>1.3277708292007446</v>
       </c>
     </row>
     <row r="61">
@@ -737,10 +737,10 @@
         <v>2009.23291015625</v>
       </c>
       <c r="B61" s="0">
-        <v>1.5678664445877075</v>
+        <v>1.8814398050308228</v>
       </c>
       <c r="C61" s="0">
-        <v>1.7098473310470581</v>
+        <v>1.7079257965087891</v>
       </c>
     </row>
     <row r="62">
@@ -748,10 +748,10 @@
         <v>2310.129638671875</v>
       </c>
       <c r="B62" s="0">
-        <v>1.5559033155441284</v>
+        <v>1.86708402633667</v>
       </c>
       <c r="C62" s="0">
-        <v>2.0119881629943848</v>
+        <v>2.0817947387695313</v>
       </c>
     </row>
     <row r="63">
@@ -759,10 +759,10 @@
         <v>2656.087890625</v>
       </c>
       <c r="B63" s="0">
-        <v>2.3273088932037354</v>
+        <v>1.6824629306793213</v>
       </c>
       <c r="C63" s="0">
-        <v>2.6399664878845215</v>
+        <v>2.3649694919586182</v>
       </c>
     </row>
     <row r="64">
@@ -770,10 +770,10 @@
         <v>3053.855712890625</v>
       </c>
       <c r="B64" s="0">
-        <v>3.8529496192932129</v>
+        <v>1.4062883853912354</v>
       </c>
       <c r="C64" s="0">
-        <v>6.3815855979919434</v>
+        <v>2.4514586925506592</v>
       </c>
     </row>
     <row r="65">
@@ -781,10 +781,10 @@
         <v>3511.19189453125</v>
       </c>
       <c r="B65" s="0">
-        <v>5.500056266784668</v>
+        <v>1.1213099956512451</v>
       </c>
       <c r="C65" s="0">
-        <v>10.916555404663086</v>
+        <v>2.2722933292388916</v>
       </c>
     </row>
     <row r="66">
@@ -792,10 +792,10 @@
         <v>4037.017333984375</v>
       </c>
       <c r="B66" s="0">
-        <v>6.4764842987060547</v>
+        <v>0.837727427482605</v>
       </c>
       <c r="C66" s="0">
-        <v>13.9111967086792</v>
+        <v>1.8533576726913452</v>
       </c>
     </row>
     <row r="67">
@@ -803,10 +803,10 @@
         <v>4641.5888671875</v>
       </c>
       <c r="B67" s="0">
-        <v>6.2729930877685547</v>
+        <v>0.567320704460144</v>
       </c>
       <c r="C67" s="0">
-        <v>14.021968841552734</v>
+        <v>1.2685675621032715</v>
       </c>
     </row>
     <row r="68">
@@ -814,10 +814,10 @@
         <v>5336.69921875</v>
       </c>
       <c r="B68" s="0">
-        <v>4.8783183097839355</v>
+        <v>0.32230293750762939</v>
       </c>
       <c r="C68" s="0">
-        <v>11.175663948059082</v>
+        <v>0.66315603256225586</v>
       </c>
     </row>
     <row r="69">
@@ -825,10 +825,10 @@
         <v>6135.9072265625</v>
       </c>
       <c r="B69" s="0">
-        <v>2.8483603000640869</v>
+        <v>0.17106030881404877</v>
       </c>
       <c r="C69" s="0">
-        <v>6.5614557266235352</v>
+        <v>0.237416610121727</v>
       </c>
     </row>
     <row r="70">
@@ -836,10 +836,10 @@
         <v>7054.80224609375</v>
       </c>
       <c r="B70" s="0">
-        <v>1.0397837162017822</v>
+        <v>0.14556881785392761</v>
       </c>
       <c r="C70" s="0">
-        <v>2.2096340656280518</v>
+        <v>0.32550176978111267</v>
       </c>
     </row>
     <row r="71">
@@ -847,10 +847,10 @@
         <v>8111.30859375</v>
       </c>
       <c r="B71" s="0">
-        <v>0.17343857884407043</v>
+        <v>0.20812630653381348</v>
       </c>
       <c r="C71" s="0">
-        <v>0.42483606934547424</v>
+        <v>0.46538460254669189</v>
       </c>
     </row>
     <row r="72">
@@ -858,10 +858,10 @@
         <v>9326.033203125</v>
       </c>
       <c r="B72" s="0">
-        <v>0.1983480304479599</v>
+        <v>0.23801761865615845</v>
       </c>
       <c r="C72" s="0">
-        <v>0.48585143685340881</v>
+        <v>0.53222358226776123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>